<commit_message>
Remove no loner needed files
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/08-various-bounds.xlsx
+++ b/ampl-data-input-excel/08-various-bounds.xlsx
@@ -267,7 +267,7 @@
     <t xml:space="preserve">2024-12-15</t>
   </si>
   <si>
-    <t xml:space="preserve">scip</t>
+    <t xml:space="preserve">highs</t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>